<commit_message>
Layout Production files for release.  BOM/ECO changes.
</commit_message>
<xml_diff>
--- a/MOUNTA.45/production files/MOUNTA.45.BOM.xlsx
+++ b/MOUNTA.45/production files/MOUNTA.45.BOM.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Designer\Documents\GitHub\MOUNTA\MOUNTA.45\production files\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Designer\Documents\GitHub\MOUNTA\MOUNTA.45\Production Files\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -19,20 +19,14 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="19">
   <si>
     <t>Product Name:</t>
   </si>
   <si>
-    <t>Mounting Bracket A 45 degree  (VER 1.0 REV A)</t>
-  </si>
-  <si>
     <t>Tag:</t>
   </si>
   <si>
-    <t>MOUNTA.45.v1.0</t>
-  </si>
-  <si>
     <t>Product Number:</t>
   </si>
   <si>
@@ -79,6 +73,9 @@
   </si>
   <si>
     <t>MOUNTA.45.v1.1</t>
+  </si>
+  <si>
+    <t>Mounting Bracket A 45 degree  (VER 1.1 REV A)</t>
   </si>
 </sst>
 </file>
@@ -472,7 +469,7 @@
   <dimension ref="A1:AMK24"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="A7" sqref="A7:XFD7"/>
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -489,20 +486,20 @@
     <col min="257" max="1025" width="8.19921875" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:13" ht="55.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="3"/>
       <c r="B1" s="4" t="s">
         <v>0</v>
       </c>
       <c r="C1" s="5" t="s">
-        <v>1</v>
+        <v>18</v>
       </c>
       <c r="D1" s="6"/>
       <c r="E1" s="4" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F1" s="5" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="G1" s="6"/>
       <c r="H1" s="6"/>
@@ -515,14 +512,14 @@
     <row r="2" spans="1:13" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="3"/>
       <c r="B2" s="4" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="C2" s="7" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="D2" s="6"/>
       <c r="E2" s="4" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="F2" s="8">
         <v>42145</v>
@@ -541,10 +538,10 @@
       <c r="C3" s="6"/>
       <c r="D3" s="6"/>
       <c r="E3" s="4" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="F3" s="8">
-        <v>42145</v>
+        <v>42397</v>
       </c>
       <c r="G3" s="6"/>
       <c r="H3" s="6"/>
@@ -586,28 +583,28 @@
     </row>
     <row r="6" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="B6" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="C6" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="B6" s="4" t="s">
+      <c r="D6" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="C6" s="4" t="s">
+      <c r="E6" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="D6" s="4" t="s">
+      <c r="F6" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="E6" s="4" t="s">
+      <c r="G6" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="F6" s="4" t="s">
+      <c r="H6" s="4" t="s">
         <v>13</v>
-      </c>
-      <c r="G6" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="H6" s="4" t="s">
-        <v>15</v>
       </c>
       <c r="I6" s="9"/>
       <c r="J6" s="3"/>
@@ -620,25 +617,25 @@
         <v>2</v>
       </c>
       <c r="B7" s="6" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="C7" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="D7" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="E7" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="F7" s="8">
+        <v>42397</v>
+      </c>
+      <c r="G7" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="H7" s="6" t="s">
         <v>16</v>
-      </c>
-      <c r="D7" s="6" t="s">
-        <v>5</v>
-      </c>
-      <c r="E7" s="5" t="s">
-        <v>3</v>
-      </c>
-      <c r="F7" s="8">
-        <v>42145</v>
-      </c>
-      <c r="G7" s="6" t="s">
-        <v>17</v>
-      </c>
-      <c r="H7" s="6" t="s">
-        <v>18</v>
       </c>
       <c r="I7" s="6"/>
       <c r="J7" s="3"/>

</xml_diff>